<commit_message>
Added support for Bexsero and Trumenba Mening B
</commit_message>
<xml_diff>
--- a/src/org/tch/forecast/core/api/impl/cvxCodes.xlsx
+++ b/src/org/tch/forecast/core/api/impl/cvxCodes.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\forecast\forecaster\src\org\tch\forecast\core\api\impl\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10836"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10830"/>
   </bookViews>
   <sheets>
     <sheet name="cvxCodes" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="507">
   <si>
     <t>CVX Label</t>
   </si>
@@ -1546,8 +1541,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2064,7 +2059,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2084,10 +2079,11 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2189,7 +2185,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2224,7 +2220,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2401,48 +2397,48 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W169"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:W171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="51.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.88671875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="11" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="4.33203125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="8.33203125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="4.28515625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="20" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="37" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="18.21875" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="35.33203125" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="17.77734375" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="35.33203125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="35.28515625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="35.28515625" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="5" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="9.6640625" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="11.6640625" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="10.109375" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="20.88671875" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="35.33203125" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="10.6640625" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="6.88671875" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="10.140625" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="20.85546875" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="35.28515625" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="6.85546875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2513,7 +2509,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23">
       <c r="A2" s="8" t="s">
         <v>363</v>
       </c>
@@ -2530,7 +2526,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23">
       <c r="A3" s="8" t="s">
         <v>379</v>
       </c>
@@ -2547,50 +2543,60 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23">
       <c r="A4" s="8" t="s">
         <v>408</v>
       </c>
       <c r="B4" s="8">
         <v>163</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C4" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="D4" s="8">
+        <v>216</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
       <c r="A5" s="8" t="s">
         <v>410</v>
       </c>
       <c r="B5" s="8">
         <v>162</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C5" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="D5" s="8">
+        <v>215</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
       <c r="A6" s="8" t="s">
         <v>412</v>
       </c>
       <c r="B6" s="8">
         <v>164</v>
       </c>
-      <c r="C6" s="8"/>
+      <c r="C6" s="8" t="s">
+        <v>412</v>
+      </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23">
       <c r="A7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>498</v>
       </c>
       <c r="C7" t="s">
@@ -2606,11 +2612,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23">
       <c r="A8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>499</v>
       </c>
       <c r="C8" t="s">
@@ -2632,11 +2638,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23">
       <c r="A9" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>500</v>
       </c>
       <c r="C9" t="s">
@@ -2667,11 +2673,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23">
       <c r="A10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>501</v>
       </c>
       <c r="C10" t="s">
@@ -2702,11 +2708,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23">
       <c r="A11" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>502</v>
       </c>
       <c r="C11" t="s">
@@ -2737,11 +2743,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23">
       <c r="A12" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>503</v>
       </c>
       <c r="C12" t="s">
@@ -2772,11 +2778,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23">
       <c r="A13" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>504</v>
       </c>
       <c r="C13" t="s">
@@ -2807,11 +2813,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23">
       <c r="A14" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>505</v>
       </c>
       <c r="C14" t="s">
@@ -2827,11 +2833,11 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23">
       <c r="A15" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>506</v>
       </c>
       <c r="C15" t="s">
@@ -2847,7 +2853,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -2867,7 +2873,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -2884,7 +2890,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -2901,7 +2907,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -2918,7 +2924,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22">
       <c r="A20" t="s">
         <v>55</v>
       </c>
@@ -2935,7 +2941,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22">
       <c r="A21" t="s">
         <v>57</v>
       </c>
@@ -2955,7 +2961,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -2975,7 +2981,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22">
       <c r="A23" t="s">
         <v>62</v>
       </c>
@@ -2995,7 +3001,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22">
       <c r="A24" t="s">
         <v>64</v>
       </c>
@@ -3012,7 +3018,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -3029,7 +3035,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22">
       <c r="A26" t="s">
         <v>67</v>
       </c>
@@ -3049,7 +3055,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22">
       <c r="A27" t="s">
         <v>68</v>
       </c>
@@ -3081,7 +3087,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22">
       <c r="A28" t="s">
         <v>70</v>
       </c>
@@ -3104,7 +3110,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22">
       <c r="A29" t="s">
         <v>72</v>
       </c>
@@ -3121,7 +3127,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22">
       <c r="A30" t="s">
         <v>73</v>
       </c>
@@ -3138,7 +3144,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22">
       <c r="A31" t="s">
         <v>74</v>
       </c>
@@ -3155,7 +3161,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22">
       <c r="A32" t="s">
         <v>75</v>
       </c>
@@ -3172,7 +3178,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23">
       <c r="A33" t="s">
         <v>76</v>
       </c>
@@ -3189,7 +3195,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23">
       <c r="A34" t="s">
         <v>77</v>
       </c>
@@ -3209,7 +3215,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23">
       <c r="A35" t="s">
         <v>79</v>
       </c>
@@ -3226,7 +3232,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:23">
       <c r="A36" t="s">
         <v>80</v>
       </c>
@@ -3243,7 +3249,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:23">
       <c r="A37" t="s">
         <v>81</v>
       </c>
@@ -3263,7 +3269,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:23">
       <c r="A38" t="s">
         <v>83</v>
       </c>
@@ -3283,7 +3289,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:23">
       <c r="A39" t="s">
         <v>86</v>
       </c>
@@ -3303,7 +3309,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:23">
       <c r="A40" t="s">
         <v>88</v>
       </c>
@@ -3320,7 +3326,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:23">
       <c r="A41" t="s">
         <v>89</v>
       </c>
@@ -3337,7 +3343,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:23">
       <c r="A42" t="s">
         <v>91</v>
       </c>
@@ -3357,7 +3363,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:23">
       <c r="A43" t="s">
         <v>92</v>
       </c>
@@ -3392,7 +3398,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:23">
       <c r="A44" t="s">
         <v>94</v>
       </c>
@@ -3427,7 +3433,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:23">
       <c r="A45" t="s">
         <v>98</v>
       </c>
@@ -3444,7 +3450,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:23">
       <c r="A46" t="s">
         <v>100</v>
       </c>
@@ -3476,7 +3482,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:23">
       <c r="A47" t="s">
         <v>101</v>
       </c>
@@ -3493,7 +3499,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:23">
       <c r="A48" t="s">
         <v>102</v>
       </c>
@@ -3513,7 +3519,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11">
       <c r="A49" t="s">
         <v>104</v>
       </c>
@@ -3533,7 +3539,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11">
       <c r="A50" t="s">
         <v>106</v>
       </c>
@@ -3553,7 +3559,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11">
       <c r="A51" t="s">
         <v>108</v>
       </c>
@@ -3573,7 +3579,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11">
       <c r="A52" t="s">
         <v>110</v>
       </c>
@@ -3593,7 +3599,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11">
       <c r="A53" t="s">
         <v>112</v>
       </c>
@@ -3613,7 +3619,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11">
       <c r="A54" t="s">
         <v>113</v>
       </c>
@@ -3633,7 +3639,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11">
       <c r="A55" t="s">
         <v>114</v>
       </c>
@@ -3653,7 +3659,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11">
       <c r="A56" t="s">
         <v>116</v>
       </c>
@@ -3676,7 +3682,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11">
       <c r="A57" t="s">
         <v>118</v>
       </c>
@@ -3699,7 +3705,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11">
       <c r="A58" t="s">
         <v>120</v>
       </c>
@@ -3719,7 +3725,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11">
       <c r="A59" t="s">
         <v>121</v>
       </c>
@@ -3736,7 +3742,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11">
       <c r="A60" t="s">
         <v>123</v>
       </c>
@@ -3753,7 +3759,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11">
       <c r="A61" t="s">
         <v>124</v>
       </c>
@@ -3770,7 +3776,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11">
       <c r="A62" t="s">
         <v>125</v>
       </c>
@@ -3787,7 +3793,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11">
       <c r="A63" t="s">
         <v>126</v>
       </c>
@@ -3804,7 +3810,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11">
       <c r="A64" t="s">
         <v>127</v>
       </c>
@@ -3815,7 +3821,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20">
       <c r="A65" t="s">
         <v>128</v>
       </c>
@@ -3832,7 +3838,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20">
       <c r="A66" t="s">
         <v>129</v>
       </c>
@@ -3849,7 +3855,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20">
       <c r="A67" t="s">
         <v>130</v>
       </c>
@@ -3860,7 +3866,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20">
       <c r="A68" t="s">
         <v>131</v>
       </c>
@@ -3880,7 +3886,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20">
       <c r="A69" t="s">
         <v>133</v>
       </c>
@@ -3891,7 +3897,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20">
       <c r="A70" t="s">
         <v>134</v>
       </c>
@@ -3908,7 +3914,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20">
       <c r="A71" t="s">
         <v>135</v>
       </c>
@@ -3925,7 +3931,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20">
       <c r="A72" t="s">
         <v>136</v>
       </c>
@@ -3942,7 +3948,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20">
       <c r="A73" t="s">
         <v>137</v>
       </c>
@@ -3959,7 +3965,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20">
       <c r="A74" t="s">
         <v>138</v>
       </c>
@@ -3976,7 +3982,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20">
       <c r="A75" t="s">
         <v>139</v>
       </c>
@@ -3993,7 +3999,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20">
       <c r="A76" t="s">
         <v>140</v>
       </c>
@@ -4010,7 +4016,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20">
       <c r="A77" t="s">
         <v>141</v>
       </c>
@@ -4027,7 +4033,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:20">
       <c r="A78" t="s">
         <v>142</v>
       </c>
@@ -4044,7 +4050,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20">
       <c r="A79" t="s">
         <v>143</v>
       </c>
@@ -4061,7 +4067,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:20">
       <c r="A80" t="s">
         <v>144</v>
       </c>
@@ -4081,7 +4087,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:23">
       <c r="A81" t="s">
         <v>147</v>
       </c>
@@ -4098,7 +4104,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:23">
       <c r="A82" t="s">
         <v>149</v>
       </c>
@@ -4115,7 +4121,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:23">
       <c r="A83" t="s">
         <v>150</v>
       </c>
@@ -4132,7 +4138,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:23">
       <c r="A84" t="s">
         <v>151</v>
       </c>
@@ -4149,7 +4155,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:23">
       <c r="A85" t="s">
         <v>152</v>
       </c>
@@ -4166,7 +4172,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:23">
       <c r="A86" t="s">
         <v>153</v>
       </c>
@@ -4198,7 +4204,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:23">
       <c r="A87" t="s">
         <v>154</v>
       </c>
@@ -4215,7 +4221,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:23">
       <c r="A88" t="s">
         <v>155</v>
       </c>
@@ -4232,7 +4238,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:23">
       <c r="A89" t="s">
         <v>157</v>
       </c>
@@ -4252,7 +4258,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:23">
       <c r="A90" t="s">
         <v>158</v>
       </c>
@@ -4272,7 +4278,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:23">
       <c r="A91" t="s">
         <v>159</v>
       </c>
@@ -4292,7 +4298,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:23">
       <c r="A92" t="s">
         <v>160</v>
       </c>
@@ -4309,7 +4315,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:23">
       <c r="A93" t="s">
         <v>161</v>
       </c>
@@ -4326,7 +4332,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:23">
       <c r="A94" t="s">
         <v>162</v>
       </c>
@@ -4346,7 +4352,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:23">
       <c r="A95" t="s">
         <v>163</v>
       </c>
@@ -4366,7 +4372,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:23">
       <c r="A96" t="s">
         <v>164</v>
       </c>
@@ -4383,7 +4389,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="97" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:22">
       <c r="A97" t="s">
         <v>165</v>
       </c>
@@ -4400,7 +4406,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="98" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:22">
       <c r="A98" t="s">
         <v>167</v>
       </c>
@@ -4417,7 +4423,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="99" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:22">
       <c r="A99" t="s">
         <v>169</v>
       </c>
@@ -4434,7 +4440,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="100" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:22">
       <c r="A100" t="s">
         <v>170</v>
       </c>
@@ -4466,7 +4472,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="101" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:22">
       <c r="A101" t="s">
         <v>172</v>
       </c>
@@ -4483,7 +4489,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="102" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:22">
       <c r="A102" t="s">
         <v>173</v>
       </c>
@@ -4500,7 +4506,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="103" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:22">
       <c r="A103" t="s">
         <v>174</v>
       </c>
@@ -4517,7 +4523,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="104" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:22">
       <c r="A104" t="s">
         <v>175</v>
       </c>
@@ -4534,7 +4540,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="105" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:22">
       <c r="A105" t="s">
         <v>177</v>
       </c>
@@ -4545,7 +4551,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="106" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:22">
       <c r="A106" t="s">
         <v>178</v>
       </c>
@@ -4568,7 +4574,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="107" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:22">
       <c r="A107" t="s">
         <v>182</v>
       </c>
@@ -4585,7 +4591,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="108" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:22">
       <c r="A108" t="s">
         <v>183</v>
       </c>
@@ -4608,7 +4614,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="109" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:22">
       <c r="A109" t="s">
         <v>185</v>
       </c>
@@ -4625,7 +4631,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="110" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:22">
       <c r="A110" t="s">
         <v>187</v>
       </c>
@@ -4648,7 +4654,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="111" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:22">
       <c r="A111" t="s">
         <v>189</v>
       </c>
@@ -4659,7 +4665,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="112" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:22">
       <c r="A112" t="s">
         <v>190</v>
       </c>
@@ -4679,7 +4685,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="113" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:23">
       <c r="A113" t="s">
         <v>191</v>
       </c>
@@ -4699,7 +4705,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="114" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:23">
       <c r="A114" t="s">
         <v>192</v>
       </c>
@@ -4719,7 +4725,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="115" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:23">
       <c r="A115" t="s">
         <v>195</v>
       </c>
@@ -4742,7 +4748,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="116" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:23">
       <c r="A116" t="s">
         <v>197</v>
       </c>
@@ -4768,7 +4774,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="117" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:23">
       <c r="A117" t="s">
         <v>199</v>
       </c>
@@ -4803,7 +4809,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="118" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:23">
       <c r="A118" t="s">
         <v>202</v>
       </c>
@@ -4814,7 +4820,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="119" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:23">
       <c r="A119" t="s">
         <v>203</v>
       </c>
@@ -4834,7 +4840,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="120" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:23">
       <c r="A120" t="s">
         <v>205</v>
       </c>
@@ -4854,7 +4860,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="121" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:23">
       <c r="A121" t="s">
         <v>208</v>
       </c>
@@ -4877,7 +4883,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="122" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:23">
       <c r="A122" t="s">
         <v>210</v>
       </c>
@@ -4897,7 +4903,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="123" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:23">
       <c r="A123" t="s">
         <v>213</v>
       </c>
@@ -4908,7 +4914,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="124" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:23">
       <c r="A124" t="s">
         <v>214</v>
       </c>
@@ -4928,7 +4934,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="125" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:23">
       <c r="A125" t="s">
         <v>216</v>
       </c>
@@ -4948,7 +4954,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="126" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:23">
       <c r="A126" t="s">
         <v>219</v>
       </c>
@@ -4974,7 +4980,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="127" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:23">
       <c r="A127" t="s">
         <v>220</v>
       </c>
@@ -4994,7 +5000,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="128" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:23">
       <c r="A128" t="s">
         <v>221</v>
       </c>
@@ -5014,7 +5020,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:19">
       <c r="A129" t="s">
         <v>223</v>
       </c>
@@ -5025,7 +5031,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:19">
       <c r="A130" t="s">
         <v>224</v>
       </c>
@@ -5045,7 +5051,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:19">
       <c r="A131" t="s">
         <v>227</v>
       </c>
@@ -5065,7 +5071,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:19">
       <c r="A132" t="s">
         <v>229</v>
       </c>
@@ -5085,7 +5091,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:19">
       <c r="A133" t="s">
         <v>231</v>
       </c>
@@ -5105,7 +5111,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:19">
       <c r="A134" t="s">
         <v>233</v>
       </c>
@@ -5116,7 +5122,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:19">
       <c r="A135" t="s">
         <v>234</v>
       </c>
@@ -5139,7 +5145,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:19">
       <c r="A136" t="s">
         <v>235</v>
       </c>
@@ -5156,7 +5162,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:19">
       <c r="A137" t="s">
         <v>237</v>
       </c>
@@ -5185,7 +5191,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:19">
       <c r="A138" t="s">
         <v>240</v>
       </c>
@@ -5208,7 +5214,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:19">
       <c r="A139" t="s">
         <v>243</v>
       </c>
@@ -5225,7 +5231,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:19">
       <c r="A140" t="s">
         <v>245</v>
       </c>
@@ -5245,7 +5251,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:19">
       <c r="A141" t="s">
         <v>247</v>
       </c>
@@ -5265,7 +5271,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="142" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:19">
       <c r="A142" t="s">
         <v>250</v>
       </c>
@@ -5285,7 +5291,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="143" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:19">
       <c r="A143" t="s">
         <v>251</v>
       </c>
@@ -5305,7 +5311,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="144" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:19">
       <c r="A144" t="s">
         <v>252</v>
       </c>
@@ -5325,7 +5331,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="145" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:19">
       <c r="A145" t="s">
         <v>253</v>
       </c>
@@ -5345,7 +5351,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="146" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:19">
       <c r="A146" t="s">
         <v>255</v>
       </c>
@@ -5365,7 +5371,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="147" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:19">
       <c r="A147" t="s">
         <v>257</v>
       </c>
@@ -5376,7 +5382,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="148" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:19">
       <c r="A148" t="s">
         <v>258</v>
       </c>
@@ -5387,7 +5393,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="149" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:19">
       <c r="A149" t="s">
         <v>259</v>
       </c>
@@ -5407,7 +5413,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="150" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:19">
       <c r="A150" t="s">
         <v>262</v>
       </c>
@@ -5418,7 +5424,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="151" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:19">
       <c r="A151" t="s">
         <v>263</v>
       </c>
@@ -5447,7 +5453,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="152" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:19">
       <c r="A152" t="s">
         <v>264</v>
       </c>
@@ -5467,7 +5473,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="153" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:19">
       <c r="A153" t="s">
         <v>265</v>
       </c>
@@ -5490,7 +5496,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="154" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:19">
       <c r="A154" t="s">
         <v>267</v>
       </c>
@@ -5510,7 +5516,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="155" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:19">
       <c r="A155" t="s">
         <v>269</v>
       </c>
@@ -5530,7 +5536,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="156" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:19">
       <c r="A156" t="s">
         <v>271</v>
       </c>
@@ -5550,7 +5556,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="157" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:19">
       <c r="A157" t="s">
         <v>272</v>
       </c>
@@ -5570,7 +5576,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="158" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:19">
       <c r="A158" t="s">
         <v>273</v>
       </c>
@@ -5584,7 +5590,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="159" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:19">
       <c r="A159" t="s">
         <v>275</v>
       </c>
@@ -5595,7 +5601,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="160" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:19">
       <c r="A160" t="s">
         <v>276</v>
       </c>
@@ -5615,7 +5621,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:12">
       <c r="A161" t="s">
         <v>277</v>
       </c>
@@ -5626,7 +5632,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:12">
       <c r="A162" t="s">
         <v>278</v>
       </c>
@@ -5637,7 +5643,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:12">
       <c r="A163" t="s">
         <v>279</v>
       </c>
@@ -5657,7 +5663,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:12">
       <c r="A164" t="s">
         <v>280</v>
       </c>
@@ -5668,7 +5674,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:12">
       <c r="A165" t="s">
         <v>281</v>
       </c>
@@ -5679,7 +5685,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:12">
       <c r="A166" t="s">
         <v>282</v>
       </c>
@@ -5696,42 +5702,76 @@
         <v>24</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:12">
       <c r="A167" t="s">
+        <v>410</v>
+      </c>
+      <c r="B167">
+        <v>215</v>
+      </c>
+      <c r="C167" t="s">
+        <v>411</v>
+      </c>
+      <c r="D167">
+        <v>162</v>
+      </c>
+      <c r="E167" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="168" spans="1:12">
+      <c r="A168" t="s">
+        <v>408</v>
+      </c>
+      <c r="B168">
+        <v>216</v>
+      </c>
+      <c r="C168" t="s">
+        <v>409</v>
+      </c>
+      <c r="D168">
+        <v>163</v>
+      </c>
+      <c r="E168" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="169" spans="1:12">
+      <c r="A169" t="s">
         <v>283</v>
       </c>
-      <c r="B167">
+      <c r="B169">
         <v>801</v>
       </c>
-      <c r="E167" t="s">
+      <c r="E169" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A168" t="s">
+    <row r="170" spans="1:12">
+      <c r="A170" t="s">
         <v>284</v>
       </c>
-      <c r="B168">
+      <c r="B170">
         <v>998</v>
       </c>
-      <c r="E168" t="s">
+      <c r="E170" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A169" t="s">
+    <row r="171" spans="1:12">
+      <c r="A171" t="s">
         <v>285</v>
       </c>
-      <c r="B169">
+      <c r="B171">
         <v>999</v>
       </c>
-      <c r="C169" t="s">
+      <c r="C171" t="s">
         <v>286</v>
       </c>
-      <c r="D169">
+      <c r="D171">
         <v>9999</v>
       </c>
-      <c r="E169" t="s">
+      <c r="E171" t="s">
         <v>52</v>
       </c>
     </row>
@@ -5742,54 +5782,54 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G167"/>
   <sheetViews>
-    <sheetView topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="G169" sqref="G169"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="51.5546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="36.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="51.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="41" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="3"/>
+    <col min="6" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:7" ht="18">
+      <c r="A1" s="10" t="s">
         <v>287</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>288</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>290</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="10" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
+    <row r="2" spans="1:7" ht="18">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
       <c r="E2" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="F2" s="9"/>
-    </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="4" t="s">
         <v>258</v>
       </c>
@@ -5809,11 +5849,11 @@
         <v>296</v>
       </c>
       <c r="G3" s="3">
-        <f>VLOOKUP(C3,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C3,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4" s="6" t="s">
         <v>123</v>
       </c>
@@ -5831,11 +5871,11 @@
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="3">
-        <f>VLOOKUP(C4,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C4,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="A5" s="4" t="s">
         <v>124</v>
       </c>
@@ -5853,11 +5893,11 @@
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="3">
-        <f>VLOOKUP(C5,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C5,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7">
       <c r="A6" s="6" t="s">
         <v>155</v>
       </c>
@@ -5877,11 +5917,11 @@
         <v>301</v>
       </c>
       <c r="G6" s="3">
-        <f>VLOOKUP(C6,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C6,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7" s="4" t="s">
         <v>73</v>
       </c>
@@ -5899,11 +5939,11 @@
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="3">
-        <f>VLOOKUP(C7,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C7,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="A8" s="6" t="s">
         <v>283</v>
       </c>
@@ -5923,11 +5963,11 @@
         <v>303</v>
       </c>
       <c r="G8" s="3">
-        <f>VLOOKUP(C8,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C8,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>801</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="A9" s="4" t="s">
         <v>66</v>
       </c>
@@ -5945,11 +5985,11 @@
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="3">
-        <f>VLOOKUP(C9,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C9,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="A10" s="6" t="s">
         <v>76</v>
       </c>
@@ -5967,11 +6007,11 @@
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="3">
-        <f>VLOOKUP(C10,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C10,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
         <v>75</v>
       </c>
@@ -5989,11 +6029,11 @@
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="3">
-        <f>VLOOKUP(C11,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C11,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7">
       <c r="A12" s="6" t="s">
         <v>79</v>
       </c>
@@ -6011,11 +6051,11 @@
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="3">
-        <f>VLOOKUP(C12,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C12,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7">
       <c r="A13" s="4" t="s">
         <v>125</v>
       </c>
@@ -6033,11 +6073,11 @@
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="3">
-        <f>VLOOKUP(C13,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C13,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7">
       <c r="A14" s="6" t="s">
         <v>53</v>
       </c>
@@ -6055,11 +6095,11 @@
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="3">
-        <f>VLOOKUP(C14,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C14,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7">
       <c r="A15" s="4" t="s">
         <v>77</v>
       </c>
@@ -6077,11 +6117,11 @@
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="3">
-        <f>VLOOKUP(C15,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C15,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7">
       <c r="A16" s="6" t="s">
         <v>67</v>
       </c>
@@ -6099,11 +6139,11 @@
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="3">
-        <f>VLOOKUP(C16,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C16,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7">
       <c r="A17" s="4" t="s">
         <v>190</v>
       </c>
@@ -6121,11 +6161,11 @@
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="3">
-        <f>VLOOKUP(C17,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C17,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7">
       <c r="A18" s="6" t="s">
         <v>191</v>
       </c>
@@ -6145,11 +6185,11 @@
         <v>313</v>
       </c>
       <c r="G18" s="3">
-        <f>VLOOKUP(C18,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C18,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7">
       <c r="A19" s="4" t="s">
         <v>263</v>
       </c>
@@ -6169,11 +6209,11 @@
         <v>316</v>
       </c>
       <c r="G19" s="3">
-        <f>VLOOKUP(C19,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C19,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7">
       <c r="A20" s="6" t="s">
         <v>197</v>
       </c>
@@ -6191,11 +6231,11 @@
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="3">
-        <f>VLOOKUP(C20,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C20,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7">
       <c r="A21" s="4" t="s">
         <v>116</v>
       </c>
@@ -6213,11 +6253,11 @@
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="3">
-        <f>VLOOKUP(C21,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C21,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7">
       <c r="A22" s="6" t="s">
         <v>219</v>
       </c>
@@ -6235,11 +6275,11 @@
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="3">
-        <f>VLOOKUP(C22,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C22,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7">
       <c r="A23" s="4" t="s">
         <v>234</v>
       </c>
@@ -6257,11 +6297,11 @@
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="3">
-        <f>VLOOKUP(C23,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C23,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>130</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7">
       <c r="A24" s="6" t="s">
         <v>237</v>
       </c>
@@ -6281,11 +6321,11 @@
         <v>322</v>
       </c>
       <c r="G24" s="3">
-        <f>VLOOKUP(C24,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C24,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>132</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7">
       <c r="A25" s="4" t="s">
         <v>323</v>
       </c>
@@ -6305,11 +6345,11 @@
         <v>325</v>
       </c>
       <c r="G25" s="3">
-        <f>VLOOKUP(C25,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C25,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>102</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7">
       <c r="A26" s="6" t="s">
         <v>23</v>
       </c>
@@ -6327,11 +6367,11 @@
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="3" t="e">
-        <f>VLOOKUP(C26,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C26,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7">
       <c r="A27" s="4" t="s">
         <v>70</v>
       </c>
@@ -6349,11 +6389,11 @@
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="3">
-        <f>VLOOKUP(C27,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C27,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7">
       <c r="A28" s="6" t="s">
         <v>126</v>
       </c>
@@ -6371,11 +6411,11 @@
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="3">
-        <f>VLOOKUP(C28,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C28,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7">
       <c r="A29" s="4" t="s">
         <v>80</v>
       </c>
@@ -6393,11 +6433,11 @@
       </c>
       <c r="F29" s="4"/>
       <c r="G29" s="3">
-        <f>VLOOKUP(C29,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C29,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7">
       <c r="A30" s="6" t="s">
         <v>120</v>
       </c>
@@ -6415,11 +6455,11 @@
       </c>
       <c r="F30" s="6"/>
       <c r="G30" s="3">
-        <f>VLOOKUP(C30,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C30,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7">
       <c r="A31" s="4" t="s">
         <v>275</v>
       </c>
@@ -6439,11 +6479,11 @@
         <v>332</v>
       </c>
       <c r="G31" s="3">
-        <f>VLOOKUP(C31,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C31,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>154</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7">
       <c r="A32" s="6" t="s">
         <v>157</v>
       </c>
@@ -6461,11 +6501,11 @@
       </c>
       <c r="F32" s="6"/>
       <c r="G32" s="3">
-        <f>VLOOKUP(C32,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C32,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7">
       <c r="A33" s="4" t="s">
         <v>158</v>
       </c>
@@ -6485,11 +6525,11 @@
         <v>335</v>
       </c>
       <c r="G33" s="3">
-        <f>VLOOKUP(C33,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C33,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7">
       <c r="A34" s="6" t="s">
         <v>81</v>
       </c>
@@ -6509,11 +6549,11 @@
         <v>337</v>
       </c>
       <c r="G34" s="3">
-        <f>VLOOKUP(C34,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C34,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7">
       <c r="A35" s="4" t="s">
         <v>159</v>
       </c>
@@ -6533,11 +6573,11 @@
         <v>339</v>
       </c>
       <c r="G35" s="3">
-        <f>VLOOKUP(C35,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C35,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7">
       <c r="A36" s="6" t="s">
         <v>187</v>
       </c>
@@ -6555,11 +6595,11 @@
       </c>
       <c r="F36" s="6"/>
       <c r="G36" s="3">
-        <f>VLOOKUP(C36,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C36,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7">
       <c r="A37" s="4" t="s">
         <v>44</v>
       </c>
@@ -6579,11 +6619,11 @@
         <v>342</v>
       </c>
       <c r="G37" s="3" t="e">
-        <f>VLOOKUP(C37,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C37,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7">
       <c r="A38" s="6" t="s">
         <v>102</v>
       </c>
@@ -6603,11 +6643,11 @@
         <v>344</v>
       </c>
       <c r="G38" s="3">
-        <f>VLOOKUP(C38,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C38,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7">
       <c r="A39" s="4" t="s">
         <v>104</v>
       </c>
@@ -6627,11 +6667,11 @@
         <v>346</v>
       </c>
       <c r="G39" s="3">
-        <f>VLOOKUP(C39,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C39,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7">
       <c r="A40" s="6" t="s">
         <v>106</v>
       </c>
@@ -6649,11 +6689,11 @@
       </c>
       <c r="F40" s="6"/>
       <c r="G40" s="3">
-        <f>VLOOKUP(C40,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C40,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7">
       <c r="A41" s="4" t="s">
         <v>108</v>
       </c>
@@ -6673,11 +6713,11 @@
         <v>349</v>
       </c>
       <c r="G41" s="3">
-        <f>VLOOKUP(C41,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C41,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7">
       <c r="A42" s="6" t="s">
         <v>127</v>
       </c>
@@ -6695,11 +6735,11 @@
       </c>
       <c r="F42" s="6"/>
       <c r="G42" s="3">
-        <f>VLOOKUP(C42,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C42,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7">
       <c r="A43" s="4" t="s">
         <v>128</v>
       </c>
@@ -6717,11 +6757,11 @@
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="3">
-        <f>VLOOKUP(C43,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C43,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>59</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7">
       <c r="A44" s="6" t="s">
         <v>129</v>
       </c>
@@ -6739,11 +6779,11 @@
       </c>
       <c r="F44" s="6"/>
       <c r="G44" s="3">
-        <f>VLOOKUP(C44,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C44,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7">
       <c r="A45" s="4" t="s">
         <v>112</v>
       </c>
@@ -6761,11 +6801,11 @@
       </c>
       <c r="F45" s="4"/>
       <c r="G45" s="3">
-        <f>VLOOKUP(C45,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C45,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7">
       <c r="A46" s="6" t="s">
         <v>110</v>
       </c>
@@ -6783,11 +6823,11 @@
       </c>
       <c r="F46" s="6"/>
       <c r="G46" s="3">
-        <f>VLOOKUP(C46,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C46,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7">
       <c r="A47" s="4" t="s">
         <v>114</v>
       </c>
@@ -6805,11 +6845,11 @@
       </c>
       <c r="F47" s="4"/>
       <c r="G47" s="3">
-        <f>VLOOKUP(C47,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C47,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7">
       <c r="A48" s="6" t="s">
         <v>113</v>
       </c>
@@ -6827,11 +6867,11 @@
       </c>
       <c r="F48" s="6"/>
       <c r="G48" s="3">
-        <f>VLOOKUP(C48,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C48,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7">
       <c r="A49" s="4" t="s">
         <v>62</v>
       </c>
@@ -6849,11 +6889,11 @@
       </c>
       <c r="F49" s="4"/>
       <c r="G49" s="3">
-        <f>VLOOKUP(C49,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C49,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7">
       <c r="A50" s="6" t="s">
         <v>118</v>
       </c>
@@ -6871,11 +6911,11 @@
       </c>
       <c r="F50" s="6"/>
       <c r="G50" s="3">
-        <f>VLOOKUP(C50,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C50,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>51</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7">
       <c r="A51" s="4" t="s">
         <v>130</v>
       </c>
@@ -6893,11 +6933,11 @@
       </c>
       <c r="F51" s="4"/>
       <c r="G51" s="3">
-        <f>VLOOKUP(C51,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C51,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>61</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7">
       <c r="A52" s="6" t="s">
         <v>214</v>
       </c>
@@ -6915,11 +6955,11 @@
       </c>
       <c r="F52" s="6"/>
       <c r="G52" s="3">
-        <f>VLOOKUP(C52,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C52,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>118</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7">
       <c r="A53" s="4" t="s">
         <v>131</v>
       </c>
@@ -6937,11 +6977,11 @@
       </c>
       <c r="F53" s="4"/>
       <c r="G53" s="3">
-        <f>VLOOKUP(C53,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C53,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>62</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7">
       <c r="A54" s="6" t="s">
         <v>250</v>
       </c>
@@ -6961,11 +7001,11 @@
         <v>362</v>
       </c>
       <c r="G54" s="3">
-        <f>VLOOKUP(C54,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C54,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>137</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7">
       <c r="A55" s="4" t="s">
         <v>363</v>
       </c>
@@ -6983,11 +7023,11 @@
       </c>
       <c r="F55" s="4"/>
       <c r="G55" s="3">
-        <f>VLOOKUP(C55,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C55,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>165</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7">
       <c r="A56" s="6" t="s">
         <v>160</v>
       </c>
@@ -7005,11 +7045,11 @@
       </c>
       <c r="F56" s="6"/>
       <c r="G56" s="3">
-        <f>VLOOKUP(C56,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C56,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>86</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7">
       <c r="A57" s="4" t="s">
         <v>55</v>
       </c>
@@ -7027,11 +7067,11 @@
       </c>
       <c r="F57" s="4"/>
       <c r="G57" s="3">
-        <f>VLOOKUP(C57,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C57,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7">
       <c r="A58" s="6" t="s">
         <v>161</v>
       </c>
@@ -7049,11 +7089,11 @@
       </c>
       <c r="F58" s="6"/>
       <c r="G58" s="3">
-        <f>VLOOKUP(C58,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C58,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>87</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7">
       <c r="A59" s="4" t="s">
         <v>281</v>
       </c>
@@ -7073,11 +7113,11 @@
         <v>369</v>
       </c>
       <c r="G59" s="3">
-        <f>VLOOKUP(C59,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C59,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>160</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7">
       <c r="A60" s="6" t="s">
         <v>271</v>
       </c>
@@ -7097,11 +7137,11 @@
         <v>370</v>
       </c>
       <c r="G60" s="3">
-        <f>VLOOKUP(C60,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C60,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>151</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7">
       <c r="A61" s="4" t="s">
         <v>223</v>
       </c>
@@ -7119,11 +7159,11 @@
       </c>
       <c r="F61" s="4"/>
       <c r="G61" s="3">
-        <f>VLOOKUP(C61,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C61,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>123</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7">
       <c r="A62" s="6" t="s">
         <v>245</v>
       </c>
@@ -7141,11 +7181,11 @@
       </c>
       <c r="F62" s="6"/>
       <c r="G62" s="3">
-        <f>VLOOKUP(C62,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C62,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>135</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7">
       <c r="A63" s="4" t="s">
         <v>273</v>
       </c>
@@ -7165,11 +7205,11 @@
         <v>374</v>
       </c>
       <c r="G63" s="3">
-        <f>VLOOKUP(C63,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C63,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>153</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7">
       <c r="A64" s="6" t="s">
         <v>279</v>
       </c>
@@ -7189,11 +7229,11 @@
         <v>376</v>
       </c>
       <c r="G64" s="3">
-        <f>VLOOKUP(C64,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C64,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>158</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7">
       <c r="A65" s="4" t="s">
         <v>269</v>
       </c>
@@ -7213,11 +7253,11 @@
         <v>378</v>
       </c>
       <c r="G65" s="3">
-        <f>VLOOKUP(C65,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C65,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>150</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7">
       <c r="A66" s="6" t="s">
         <v>282</v>
       </c>
@@ -7235,11 +7275,11 @@
       </c>
       <c r="F66" s="6"/>
       <c r="G66" s="3">
-        <f>VLOOKUP(C66,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C66,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>161</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7">
       <c r="A67" s="4" t="s">
         <v>379</v>
       </c>
@@ -7257,11 +7297,11 @@
       </c>
       <c r="F67" s="4"/>
       <c r="G67" s="3">
-        <f>VLOOKUP(C67,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C67,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>166</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7">
       <c r="A68" s="6" t="s">
         <v>199</v>
       </c>
@@ -7281,11 +7321,11 @@
         <v>382</v>
       </c>
       <c r="G68" s="3">
-        <f>VLOOKUP(C68,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C68,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>111</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7">
       <c r="A69" s="4" t="s">
         <v>267</v>
       </c>
@@ -7305,11 +7345,11 @@
         <v>383</v>
       </c>
       <c r="G69" s="3">
-        <f>VLOOKUP(C69,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C69,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>149</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7">
       <c r="A70" s="6" t="s">
         <v>276</v>
       </c>
@@ -7329,11 +7369,11 @@
         <v>385</v>
       </c>
       <c r="G70" s="3">
-        <f>VLOOKUP(C70,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C70,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>155</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7">
       <c r="A71" s="4" t="s">
         <v>255</v>
       </c>
@@ -7353,11 +7393,11 @@
         <v>386</v>
       </c>
       <c r="G71" s="3">
-        <f>VLOOKUP(C71,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C71,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>141</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7">
       <c r="A72" s="6" t="s">
         <v>253</v>
       </c>
@@ -7377,11 +7417,11 @@
         <v>387</v>
       </c>
       <c r="G72" s="3">
-        <f>VLOOKUP(C72,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C72,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>140</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7">
       <c r="A73" s="4" t="s">
         <v>259</v>
       </c>
@@ -7401,11 +7441,11 @@
         <v>389</v>
       </c>
       <c r="G73" s="3">
-        <f>VLOOKUP(C73,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C73,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>144</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7">
       <c r="A74" s="6" t="s">
         <v>57</v>
       </c>
@@ -7425,11 +7465,11 @@
         <v>391</v>
       </c>
       <c r="G74" s="3">
-        <f>VLOOKUP(C74,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C74,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7">
       <c r="A75" s="4" t="s">
         <v>162</v>
       </c>
@@ -7449,11 +7489,11 @@
         <v>393</v>
       </c>
       <c r="G75" s="3">
-        <f>VLOOKUP(C75,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C75,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>88</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7">
       <c r="A76" s="6" t="s">
         <v>60</v>
       </c>
@@ -7471,11 +7511,11 @@
       </c>
       <c r="F76" s="6"/>
       <c r="G76" s="3">
-        <f>VLOOKUP(C76,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C76,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7">
       <c r="A77" s="4" t="s">
         <v>49</v>
       </c>
@@ -7493,11 +7533,11 @@
       </c>
       <c r="F77" s="4"/>
       <c r="G77" s="3">
-        <f>VLOOKUP(C77,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C77,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7">
       <c r="A78" s="6" t="s">
         <v>243</v>
       </c>
@@ -7515,11 +7555,11 @@
       </c>
       <c r="F78" s="6"/>
       <c r="G78" s="3">
-        <f>VLOOKUP(C78,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C78,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>134</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7">
       <c r="A79" s="4" t="s">
         <v>98</v>
       </c>
@@ -7537,11 +7577,11 @@
       </c>
       <c r="F79" s="4"/>
       <c r="G79" s="3">
-        <f>VLOOKUP(C79,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C79,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>39</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7">
       <c r="A80" s="6" t="s">
         <v>233</v>
       </c>
@@ -7561,11 +7601,11 @@
         <v>399</v>
       </c>
       <c r="G80" s="3">
-        <f>VLOOKUP(C80,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C80,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>129</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7">
       <c r="A81" s="4" t="s">
         <v>133</v>
       </c>
@@ -7583,11 +7623,11 @@
       </c>
       <c r="F81" s="4"/>
       <c r="G81" s="3">
-        <f>VLOOKUP(C81,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C81,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>63</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7">
       <c r="A82" s="6" t="s">
         <v>134</v>
       </c>
@@ -7605,11 +7645,11 @@
       </c>
       <c r="F82" s="6"/>
       <c r="G82" s="3">
-        <f>VLOOKUP(C82,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C82,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>64</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7">
       <c r="A83" s="4" t="s">
         <v>135</v>
       </c>
@@ -7627,11 +7667,11 @@
       </c>
       <c r="F83" s="4"/>
       <c r="G83" s="3">
-        <f>VLOOKUP(C83,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C83,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>65</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7">
       <c r="A84" s="6" t="s">
         <v>136</v>
       </c>
@@ -7649,11 +7689,11 @@
       </c>
       <c r="F84" s="6"/>
       <c r="G84" s="3">
-        <f>VLOOKUP(C84,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C84,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>66</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7">
       <c r="A85" s="4" t="s">
         <v>32</v>
       </c>
@@ -7671,11 +7711,11 @@
       </c>
       <c r="F85" s="4"/>
       <c r="G85" s="3" t="e">
-        <f>VLOOKUP(C85,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C85,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7">
       <c r="A86" s="6" t="s">
         <v>137</v>
       </c>
@@ -7693,11 +7733,11 @@
       </c>
       <c r="F86" s="6"/>
       <c r="G86" s="3">
-        <f>VLOOKUP(C86,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C86,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>67</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7">
       <c r="A87" s="4" t="s">
         <v>35</v>
       </c>
@@ -7715,11 +7755,11 @@
       </c>
       <c r="F87" s="4"/>
       <c r="G87" s="3" t="e">
-        <f>VLOOKUP(C87,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C87,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7">
       <c r="A88" s="6" t="s">
         <v>138</v>
       </c>
@@ -7737,11 +7777,11 @@
       </c>
       <c r="F88" s="6"/>
       <c r="G88" s="3">
-        <f>VLOOKUP(C88,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C88,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>68</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7">
       <c r="A89" s="4" t="s">
         <v>408</v>
       </c>
@@ -7759,11 +7799,11 @@
       </c>
       <c r="F89" s="4"/>
       <c r="G89" s="3">
-        <f>VLOOKUP(C89,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C89,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>163</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7">
       <c r="A90" s="6" t="s">
         <v>410</v>
       </c>
@@ -7781,11 +7821,11 @@
       </c>
       <c r="F90" s="6"/>
       <c r="G90" s="3">
-        <f>VLOOKUP(C90,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C90,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>162</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7">
       <c r="A91" s="4" t="s">
         <v>412</v>
       </c>
@@ -7803,11 +7843,11 @@
       </c>
       <c r="F91" s="4"/>
       <c r="G91" s="3">
-        <f>VLOOKUP(C91,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C91,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>164</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7">
       <c r="A92" s="6" t="s">
         <v>185</v>
       </c>
@@ -7825,11 +7865,11 @@
       </c>
       <c r="F92" s="6"/>
       <c r="G92" s="3">
-        <f>VLOOKUP(C92,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C92,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>103</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7">
       <c r="A93" s="4" t="s">
         <v>265</v>
       </c>
@@ -7847,11 +7887,11 @@
       </c>
       <c r="F93" s="4"/>
       <c r="G93" s="3">
-        <f>VLOOKUP(C93,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C93,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>148</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7">
       <c r="A94" s="6" t="s">
         <v>264</v>
       </c>
@@ -7871,11 +7911,11 @@
         <v>417</v>
       </c>
       <c r="G94" s="3">
-        <f>VLOOKUP(C94,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C94,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>147</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7">
       <c r="A95" s="4" t="s">
         <v>247</v>
       </c>
@@ -7893,11 +7933,11 @@
       </c>
       <c r="F95" s="4"/>
       <c r="G95" s="3">
-        <f>VLOOKUP(C95,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C95,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>136</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7">
       <c r="A96" s="6" t="s">
         <v>205</v>
       </c>
@@ -7915,11 +7955,11 @@
       </c>
       <c r="F96" s="6"/>
       <c r="G96" s="3">
-        <f>VLOOKUP(C96,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C96,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>114</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7">
       <c r="A97" s="4" t="s">
         <v>83</v>
       </c>
@@ -7937,11 +7977,11 @@
       </c>
       <c r="F97" s="4"/>
       <c r="G97" s="3">
-        <f>VLOOKUP(C97,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C97,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>32</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7">
       <c r="A98" s="6" t="s">
         <v>192</v>
       </c>
@@ -7961,11 +8001,11 @@
         <v>422</v>
       </c>
       <c r="G98" s="3">
-        <f>VLOOKUP(C98,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C98,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>108</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7">
       <c r="A99" s="4" t="s">
         <v>30</v>
       </c>
@@ -7983,11 +8023,11 @@
       </c>
       <c r="F99" s="4"/>
       <c r="G99" s="3" t="e">
-        <f>VLOOKUP(C99,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C99,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7">
       <c r="A100" s="6" t="s">
         <v>170</v>
       </c>
@@ -8005,11 +8045,11 @@
       </c>
       <c r="F100" s="6"/>
       <c r="G100" s="3">
-        <f>VLOOKUP(C100,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C100,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>94</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7">
       <c r="A101" s="4" t="s">
         <v>41</v>
       </c>
@@ -8027,11 +8067,11 @@
       </c>
       <c r="F101" s="4"/>
       <c r="G101" s="3" t="e">
-        <f>VLOOKUP(C101,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C101,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7">
       <c r="A102" s="6" t="s">
         <v>229</v>
       </c>
@@ -8049,11 +8089,11 @@
       </c>
       <c r="F102" s="6"/>
       <c r="G102" s="3">
-        <f>VLOOKUP(C102,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C102,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>127</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7">
       <c r="A103" s="4" t="s">
         <v>231</v>
       </c>
@@ -8073,11 +8113,11 @@
         <v>428</v>
       </c>
       <c r="G103" s="3">
-        <f>VLOOKUP(C103,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C103,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>128</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7">
       <c r="A104" s="6" t="s">
         <v>224</v>
       </c>
@@ -8095,11 +8135,11 @@
       </c>
       <c r="F104" s="6"/>
       <c r="G104" s="3">
-        <f>VLOOKUP(C104,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C104,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>125</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7">
       <c r="A105" s="4" t="s">
         <v>227</v>
       </c>
@@ -8117,11 +8157,11 @@
       </c>
       <c r="F105" s="4"/>
       <c r="G105" s="3">
-        <f>VLOOKUP(C105,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C105,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>126</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7">
       <c r="A106" s="6" t="s">
         <v>26</v>
       </c>
@@ -8139,11 +8179,11 @@
       </c>
       <c r="F106" s="6"/>
       <c r="G106" s="3" t="e">
-        <f>VLOOKUP(C106,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C106,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7">
       <c r="A107" s="4" t="s">
         <v>139</v>
       </c>
@@ -8161,11 +8201,11 @@
       </c>
       <c r="F107" s="4"/>
       <c r="G107" s="3">
-        <f>VLOOKUP(C107,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C107,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>69</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7">
       <c r="A108" s="6" t="s">
         <v>51</v>
       </c>
@@ -8183,11 +8223,11 @@
       </c>
       <c r="F108" s="6"/>
       <c r="G108" s="3">
-        <f>VLOOKUP(C108,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C108,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7">
       <c r="A109" s="4" t="s">
         <v>72</v>
       </c>
@@ -8205,11 +8245,11 @@
       </c>
       <c r="F109" s="4"/>
       <c r="G109" s="3">
-        <f>VLOOKUP(C109,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C109,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>23</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7">
       <c r="A110" s="6" t="s">
         <v>240</v>
       </c>
@@ -8227,11 +8267,11 @@
       </c>
       <c r="F110" s="6"/>
       <c r="G110" s="3">
-        <f>VLOOKUP(C110,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C110,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>133</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7">
       <c r="A111" s="4" t="s">
         <v>178</v>
       </c>
@@ -8249,11 +8289,11 @@
       </c>
       <c r="F111" s="4"/>
       <c r="G111" s="3">
-        <f>VLOOKUP(C111,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C111,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>100</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7">
       <c r="A112" s="6" t="s">
         <v>272</v>
       </c>
@@ -8273,11 +8313,11 @@
         <v>437</v>
       </c>
       <c r="G112" s="3">
-        <f>VLOOKUP(C112,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C112,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>152</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7">
       <c r="A113" s="4" t="s">
         <v>86</v>
       </c>
@@ -8295,11 +8335,11 @@
       </c>
       <c r="F113" s="4"/>
       <c r="G113" s="3">
-        <f>VLOOKUP(C113,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C113,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>33</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7">
       <c r="A114" s="6" t="s">
         <v>195</v>
       </c>
@@ -8319,11 +8359,11 @@
         <v>440</v>
       </c>
       <c r="G114" s="3">
-        <f>VLOOKUP(C114,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C114,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>109</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7">
       <c r="A115" s="4" t="s">
         <v>163</v>
       </c>
@@ -8343,11 +8383,11 @@
         <v>442</v>
       </c>
       <c r="G115" s="3">
-        <f>VLOOKUP(C115,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C115,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>89</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7">
       <c r="A116" s="6" t="s">
         <v>140</v>
       </c>
@@ -8365,11 +8405,11 @@
       </c>
       <c r="F116" s="6"/>
       <c r="G116" s="3">
-        <f>VLOOKUP(C116,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C116,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>70</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7">
       <c r="A117" s="4" t="s">
         <v>100</v>
       </c>
@@ -8387,11 +8427,11 @@
       </c>
       <c r="F117" s="4"/>
       <c r="G117" s="3">
-        <f>VLOOKUP(C117,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C117,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>40</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7">
       <c r="A118" s="6" t="s">
         <v>64</v>
       </c>
@@ -8409,11 +8449,11 @@
       </c>
       <c r="F118" s="6"/>
       <c r="G118" s="3">
-        <f>VLOOKUP(C118,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C118,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>18</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7">
       <c r="A119" s="4" t="s">
         <v>164</v>
       </c>
@@ -8433,11 +8473,11 @@
         <v>447</v>
       </c>
       <c r="G119" s="3">
-        <f>VLOOKUP(C119,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C119,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>90</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7">
       <c r="A120" s="6" t="s">
         <v>142</v>
       </c>
@@ -8455,11 +8495,11 @@
       </c>
       <c r="F120" s="6"/>
       <c r="G120" s="3">
-        <f>VLOOKUP(C120,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C120,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>72</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7">
       <c r="A121" s="4" t="s">
         <v>280</v>
       </c>
@@ -8477,11 +8517,11 @@
       </c>
       <c r="F121" s="4"/>
       <c r="G121" s="3">
-        <f>VLOOKUP(C121,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C121,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>159</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7">
       <c r="A122" s="6" t="s">
         <v>278</v>
       </c>
@@ -8501,11 +8541,11 @@
         <v>451</v>
       </c>
       <c r="G122" s="3">
-        <f>VLOOKUP(C122,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C122,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>157</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7">
       <c r="A123" s="4" t="s">
         <v>277</v>
       </c>
@@ -8525,11 +8565,11 @@
         <v>453</v>
       </c>
       <c r="G123" s="3">
-        <f>VLOOKUP(C123,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C123,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>156</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7">
       <c r="A124" s="6" t="s">
         <v>143</v>
       </c>
@@ -8547,11 +8587,11 @@
       </c>
       <c r="F124" s="6"/>
       <c r="G124" s="3">
-        <f>VLOOKUP(C124,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C124,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>73</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7">
       <c r="A125" s="4" t="s">
         <v>88</v>
       </c>
@@ -8569,11 +8609,11 @@
       </c>
       <c r="F125" s="4"/>
       <c r="G125" s="3">
-        <f>VLOOKUP(C125,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C125,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>34</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7">
       <c r="A126" s="6" t="s">
         <v>216</v>
       </c>
@@ -8591,11 +8631,11 @@
       </c>
       <c r="F126" s="6"/>
       <c r="G126" s="3">
-        <f>VLOOKUP(C126,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C126,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>119</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7">
       <c r="A127" s="4" t="s">
         <v>210</v>
       </c>
@@ -8613,11 +8653,11 @@
       </c>
       <c r="F127" s="4"/>
       <c r="G127" s="3">
-        <f>VLOOKUP(C127,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C127,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>116</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7">
       <c r="A128" s="6" t="s">
         <v>144</v>
       </c>
@@ -8635,11 +8675,11 @@
       </c>
       <c r="F128" s="6"/>
       <c r="G128" s="3">
-        <f>VLOOKUP(C128,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C128,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>74</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7">
       <c r="A129" s="4" t="s">
         <v>221</v>
       </c>
@@ -8657,11 +8697,11 @@
       </c>
       <c r="F129" s="4"/>
       <c r="G129" s="3">
-        <f>VLOOKUP(C129,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C129,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>122</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7">
       <c r="A130" s="6" t="s">
         <v>141</v>
       </c>
@@ -8679,11 +8719,11 @@
       </c>
       <c r="F130" s="6"/>
       <c r="G130" s="3">
-        <f>VLOOKUP(C130,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C130,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>71</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7">
       <c r="A131" s="4" t="s">
         <v>169</v>
       </c>
@@ -8701,11 +8741,11 @@
       </c>
       <c r="F131" s="4"/>
       <c r="G131" s="3">
-        <f>VLOOKUP(C131,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C131,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>93</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7">
       <c r="A132" s="6" t="s">
         <v>262</v>
       </c>
@@ -8723,11 +8763,11 @@
       </c>
       <c r="F132" s="6"/>
       <c r="G132" s="3">
-        <f>VLOOKUP(C132,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C132,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>145</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7">
       <c r="A133" s="4" t="s">
         <v>38</v>
       </c>
@@ -8745,11 +8785,11 @@
       </c>
       <c r="F133" s="4"/>
       <c r="G133" s="3" t="e">
-        <f>VLOOKUP(C133,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C133,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7">
       <c r="A134" s="6" t="s">
         <v>94</v>
       </c>
@@ -8767,11 +8807,11 @@
       </c>
       <c r="F134" s="6"/>
       <c r="G134" s="3">
-        <f>VLOOKUP(C134,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C134,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>38</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7">
       <c r="A135" s="4" t="s">
         <v>149</v>
       </c>
@@ -8789,11 +8829,11 @@
       </c>
       <c r="F135" s="4"/>
       <c r="G135" s="3">
-        <f>VLOOKUP(C135,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C135,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>76</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7">
       <c r="A136" s="6" t="s">
         <v>251</v>
       </c>
@@ -8813,11 +8853,11 @@
         <v>467</v>
       </c>
       <c r="G136" s="3">
-        <f>VLOOKUP(C136,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C136,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>138</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7">
       <c r="A137" s="4" t="s">
         <v>203</v>
       </c>
@@ -8835,11 +8875,11 @@
       </c>
       <c r="F137" s="4"/>
       <c r="G137" s="3">
-        <f>VLOOKUP(C137,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C137,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>113</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7">
       <c r="A138" s="6" t="s">
         <v>46</v>
       </c>
@@ -8859,11 +8899,11 @@
         <v>470</v>
       </c>
       <c r="G138" s="3" t="e">
-        <f>VLOOKUP(C138,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C138,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7">
       <c r="A139" s="4" t="s">
         <v>252</v>
       </c>
@@ -8883,11 +8923,11 @@
         <v>471</v>
       </c>
       <c r="G139" s="3">
-        <f>VLOOKUP(C139,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C139,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>139</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7">
       <c r="A140" s="6" t="s">
         <v>208</v>
       </c>
@@ -8905,11 +8945,11 @@
       </c>
       <c r="F140" s="6"/>
       <c r="G140" s="3">
-        <f>VLOOKUP(C140,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C140,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>115</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7">
       <c r="A141" s="4" t="s">
         <v>89</v>
       </c>
@@ -8927,11 +8967,11 @@
       </c>
       <c r="F141" s="4"/>
       <c r="G141" s="3">
-        <f>VLOOKUP(C141,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C141,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>35</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7">
       <c r="A142" s="6" t="s">
         <v>257</v>
       </c>
@@ -8949,11 +8989,11 @@
       </c>
       <c r="F142" s="6"/>
       <c r="G142" s="3">
-        <f>VLOOKUP(C142,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C142,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>142</v>
       </c>
     </row>
-    <row r="143" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7">
       <c r="A143" s="4" t="s">
         <v>202</v>
       </c>
@@ -8971,11 +9011,11 @@
       </c>
       <c r="F143" s="4"/>
       <c r="G143" s="3">
-        <f>VLOOKUP(C143,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C143,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>112</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7">
       <c r="A144" s="6" t="s">
         <v>150</v>
       </c>
@@ -8993,11 +9033,11 @@
       </c>
       <c r="F144" s="6"/>
       <c r="G144" s="3">
-        <f>VLOOKUP(C144,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C144,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>77</v>
       </c>
     </row>
-    <row r="145" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7">
       <c r="A145" s="4" t="s">
         <v>54</v>
       </c>
@@ -9015,11 +9055,11 @@
       </c>
       <c r="F145" s="4"/>
       <c r="G145" s="3">
-        <f>VLOOKUP(C145,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C145,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>13</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7">
       <c r="A146" s="6" t="s">
         <v>175</v>
       </c>
@@ -9039,11 +9079,11 @@
         <v>476</v>
       </c>
       <c r="G146" s="3">
-        <f>VLOOKUP(C146,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C146,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>98</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7">
       <c r="A147" s="4" t="s">
         <v>172</v>
       </c>
@@ -9063,11 +9103,11 @@
         <v>476</v>
       </c>
       <c r="G147" s="3">
-        <f>VLOOKUP(C147,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C147,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>95</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7">
       <c r="A148" s="6" t="s">
         <v>173</v>
       </c>
@@ -9087,11 +9127,11 @@
         <v>476</v>
       </c>
       <c r="G148" s="3">
-        <f>VLOOKUP(C148,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C148,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>96</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7">
       <c r="A149" s="4" t="s">
         <v>174</v>
       </c>
@@ -9111,11 +9151,11 @@
         <v>476</v>
       </c>
       <c r="G149" s="3">
-        <f>VLOOKUP(C149,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C149,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>97</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7">
       <c r="A150" s="6" t="s">
         <v>151</v>
       </c>
@@ -9133,11 +9173,11 @@
       </c>
       <c r="F150" s="6"/>
       <c r="G150" s="3">
-        <f>VLOOKUP(C150,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C150,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>78</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7">
       <c r="A151" s="4" t="s">
         <v>74</v>
       </c>
@@ -9155,11 +9195,11 @@
       </c>
       <c r="F151" s="4"/>
       <c r="G151" s="3">
-        <f>VLOOKUP(C151,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C151,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>25</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7">
       <c r="A152" s="6" t="s">
         <v>101</v>
       </c>
@@ -9177,11 +9217,11 @@
       </c>
       <c r="F152" s="6"/>
       <c r="G152" s="3">
-        <f>VLOOKUP(C152,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C152,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>41</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7">
       <c r="A153" s="4" t="s">
         <v>121</v>
       </c>
@@ -9199,11 +9239,11 @@
       </c>
       <c r="F153" s="4"/>
       <c r="G153" s="3">
-        <f>VLOOKUP(C153,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C153,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>53</v>
       </c>
     </row>
-    <row r="154" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7">
       <c r="A154" s="6" t="s">
         <v>165</v>
       </c>
@@ -9223,11 +9263,11 @@
         <v>484</v>
       </c>
       <c r="G154" s="3">
-        <f>VLOOKUP(C154,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C154,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>91</v>
       </c>
     </row>
-    <row r="155" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:7">
       <c r="A155" s="4" t="s">
         <v>182</v>
       </c>
@@ -9245,11 +9285,11 @@
       </c>
       <c r="F155" s="4"/>
       <c r="G155" s="3">
-        <f>VLOOKUP(C155,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C155,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>101</v>
       </c>
     </row>
-    <row r="156" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7">
       <c r="A156" s="6" t="s">
         <v>235</v>
       </c>
@@ -9267,11 +9307,11 @@
       </c>
       <c r="F156" s="6"/>
       <c r="G156" s="3">
-        <f>VLOOKUP(C156,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C156,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>131</v>
       </c>
     </row>
-    <row r="157" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:7">
       <c r="A157" s="4" t="s">
         <v>147</v>
       </c>
@@ -9289,11 +9329,11 @@
       </c>
       <c r="F157" s="4"/>
       <c r="G157" s="3">
-        <f>VLOOKUP(C157,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C157,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>75</v>
       </c>
     </row>
-    <row r="158" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7">
       <c r="A158" s="6" t="s">
         <v>189</v>
       </c>
@@ -9311,11 +9351,11 @@
       </c>
       <c r="F158" s="6"/>
       <c r="G158" s="3">
-        <f>VLOOKUP(C158,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C158,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>105</v>
       </c>
     </row>
-    <row r="159" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7">
       <c r="A159" s="4" t="s">
         <v>152</v>
       </c>
@@ -9333,11 +9373,11 @@
       </c>
       <c r="F159" s="4"/>
       <c r="G159" s="3">
-        <f>VLOOKUP(C159,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C159,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>79</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:7">
       <c r="A160" s="6" t="s">
         <v>68</v>
       </c>
@@ -9355,11 +9395,11 @@
       </c>
       <c r="F160" s="6"/>
       <c r="G160" s="3">
-        <f>VLOOKUP(C160,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C160,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>21</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7">
       <c r="A161" s="4" t="s">
         <v>154</v>
       </c>
@@ -9377,11 +9417,11 @@
       </c>
       <c r="F161" s="4"/>
       <c r="G161" s="3">
-        <f>VLOOKUP(C161,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C161,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>81</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:7">
       <c r="A162" s="6" t="s">
         <v>153</v>
       </c>
@@ -9399,11 +9439,11 @@
       </c>
       <c r="F162" s="6"/>
       <c r="G162" s="3">
-        <f>VLOOKUP(C162,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C162,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>80</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:7">
       <c r="A163" s="4" t="s">
         <v>167</v>
       </c>
@@ -9423,11 +9463,11 @@
         <v>493</v>
       </c>
       <c r="G163" s="3">
-        <f>VLOOKUP(C163,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C163,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>92</v>
       </c>
     </row>
-    <row r="164" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:7">
       <c r="A164" s="6" t="s">
         <v>91</v>
       </c>
@@ -9445,11 +9485,11 @@
       </c>
       <c r="F164" s="6"/>
       <c r="G164" s="3">
-        <f>VLOOKUP(C164,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C164,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>36</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:7">
       <c r="A165" s="4" t="s">
         <v>213</v>
       </c>
@@ -9467,11 +9507,11 @@
       </c>
       <c r="F165" s="4"/>
       <c r="G165" s="3">
-        <f>VLOOKUP(C165,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C165,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>117</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:7">
       <c r="A166" s="6" t="s">
         <v>92</v>
       </c>
@@ -9489,11 +9529,11 @@
       </c>
       <c r="F166" s="6"/>
       <c r="G166" s="3">
-        <f>VLOOKUP(C166,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C166,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>37</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:7">
       <c r="A167" s="4" t="s">
         <v>220</v>
       </c>
@@ -9511,7 +9551,7 @@
       </c>
       <c r="F167" s="4"/>
       <c r="G167" s="3">
-        <f>VLOOKUP(C167,cvxCodes!B$2:B$169,1, FALSE)</f>
+        <f>VLOOKUP(C167,cvxCodes!B$2:B$171,1, FALSE)</f>
         <v>121</v>
       </c>
     </row>

</xml_diff>